<commit_message>
First pass at Squid project - works but is slow
git-svn-id: https://svn.broadinstitute.org/BTL/tracker@629 49feb11a-dc6b-4521-947f-5d0cd0a85b6f
</commit_message>
<xml_diff>
--- a/conf/data/EZPass.xlsx
+++ b/conf/data/EZPass.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="640" windowWidth="24020" windowHeight="12480"/>
+    <workbookView xWindow="740" yWindow="640" windowWidth="40480" windowHeight="18260"/>
   </bookViews>
   <sheets>
     <sheet name="New Technology Lib Kit" sheetId="1" r:id="rId1"/>
@@ -846,7 +846,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -991,6 +991,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1099,7 +1100,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="142">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="120"/>
     <cellStyle name="20% - Accent2" xfId="93" builtinId="34" customBuiltin="1"/>
@@ -1208,6 +1209,7 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="77" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="73" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="74" builtinId="17" customBuiltin="1"/>
@@ -1610,8 +1612,8 @@
   </sheetPr>
   <dimension ref="A2:AL29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2033,7 +2035,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:38" s="29" customFormat="1" ht="96">
+    <row r="29" spans="1:38" s="29" customFormat="1" ht="120">
       <c r="A29" s="30" t="s">
         <v>3</v>
       </c>
@@ -2043,110 +2045,110 @@
       <c r="C29" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="L29" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="M29" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="O29" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="P29" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="R29" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="S29" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="T29" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="U29" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="V29" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="W29" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="X29" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y29" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA29" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB29" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC29" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD29" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE29" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF29" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG29" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH29" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI29" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ29" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK29" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="43" t="s">
+      <c r="AL29" s="43" t="s">
         <v>69</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="K29" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M29" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="N29" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="O29" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="P29" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q29" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="R29" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="S29" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="T29" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="U29" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="V29" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="W29" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="X29" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y29" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z29" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA29" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC29" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD29" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE29" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF29" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG29" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH29" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI29" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ29" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK29" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL29" s="35" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix up spreadsheet comments, speed up EZPass creation to around 5 seconds for 96 sample tube, get rid of Await.results calls (they're ugly)
git-svn-id: https://svn.broadinstitute.org/BTL/tracker@637 49feb11a-dc6b-4521-947f-5d0cd0a85b6f
</commit_message>
<xml_diff>
--- a/conf/data/EZPass.xlsx
+++ b/conf/data/EZPass.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="640" windowWidth="40480" windowHeight="18260"/>
+    <workbookView xWindow="3540" yWindow="220" windowWidth="40480" windowHeight="18260"/>
   </bookViews>
   <sheets>
     <sheet name="New Technology Lib Kit" sheetId="1" r:id="rId1"/>
@@ -485,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -699,6 +699,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -993,7 +999,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1099,6 +1105,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="142">
     <cellStyle name="20% - Accent1" xfId="89" builtinId="30" customBuiltin="1"/>
@@ -1612,17 +1619,21 @@
   </sheetPr>
   <dimension ref="A2:AL29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" style="7" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
-    <col min="3" max="5" width="15.5" style="41" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="41" customWidth="1"/>
+    <col min="4" max="4" width="39" style="41" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="41" customWidth="1"/>
     <col min="6" max="6" width="38.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="7.5" style="7" customWidth="1"/>
+    <col min="7" max="8" width="7.5" style="7" customWidth="1"/>
+    <col min="9" max="9" width="26.5" style="7" customWidth="1"/>
+    <col min="10" max="10" width="28.83203125" style="7" customWidth="1"/>
     <col min="11" max="11" width="46.5" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="34.5" style="7" customWidth="1"/>
     <col min="13" max="13" width="48.33203125" style="7" customWidth="1"/>
@@ -1632,12 +1643,14 @@
     <col min="17" max="19" width="20.5" style="7" customWidth="1"/>
     <col min="20" max="20" width="9.5" style="7" customWidth="1"/>
     <col min="21" max="21" width="25.33203125" style="7" customWidth="1"/>
-    <col min="22" max="24" width="8.6640625" style="7" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" style="7" customWidth="1"/>
+    <col min="23" max="23" width="25.83203125" style="7" customWidth="1"/>
+    <col min="24" max="24" width="28.5" style="7" customWidth="1"/>
     <col min="25" max="25" width="23.5" style="7" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="31.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="19.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.5" style="7" customWidth="1"/>
+    <col min="28" max="28" width="25.1640625" style="7" customWidth="1"/>
+    <col min="29" max="29" width="31" style="7" customWidth="1"/>
     <col min="30" max="30" width="25.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="48.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.5" style="7" bestFit="1" customWidth="1"/>
@@ -1959,10 +1972,6 @@
       <c r="B24" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="AA24" s="7">
-        <f>((20/10^9)/0.001)*(650*390)</f>
-        <v>5.07</v>
-      </c>
     </row>
     <row r="25" spans="1:38" ht="24">
       <c r="B25" s="26" t="s">
@@ -1982,36 +1991,41 @@
       <c r="B28" s="28"/>
       <c r="C28" s="42"/>
       <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="G28" s="7" t="s">
+      <c r="E28" s="41" t="s">
         <v>58</v>
       </c>
+      <c r="I28" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="K28" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="P28" s="36" t="s">
+      <c r="N28" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="R28" s="7" t="s">
+      <c r="P28" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="U28" s="7" t="s">
+      <c r="S28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="Y28" s="7" t="s">
+      <c r="W28" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="Z28" s="7" t="s">
+      <c r="X28" s="7" t="s">
         <v>64</v>
       </c>
+      <c r="AC28" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD28" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="AE28" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AF28" s="7" t="s">
         <v>61</v>
@@ -2028,14 +2042,8 @@
       <c r="AJ28" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AK28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL28" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" s="29" customFormat="1" ht="120">
+    </row>
+    <row r="29" spans="1:38" s="29" customFormat="1" ht="60">
       <c r="A29" s="30" t="s">
         <v>3</v>
       </c>

</xml_diff>